<commit_message>
PCB Final ahora sí
</commit_message>
<xml_diff>
--- a/PCB/PCB_Project/Project Outputs for TP2-FlyBack/TP2-FlyBack.xlsx
+++ b/PCB/PCB_Project/Project Outputs for TP2-FlyBack/TP2-FlyBack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00 - ITBA\Electrónica 4\Trabajos Prácticos\TP2-Flyback\TP2-FlyBack\PCB\PCB_Project\Project Outputs for TP2-FlyBack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E164EA39-3021-411D-937C-87344BCB2D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9083EBC7-838C-451C-B4AC-F0336E66BA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14610" windowHeight="15225" xr2:uid="{B9BFC7E0-D1B2-4A23-BDA8-1F5E5EED93C1}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="11295" xr2:uid="{37B77970-8D77-41D0-9994-FF57F0FF287E}"/>
   </bookViews>
   <sheets>
     <sheet name="TP2-FlyBack" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="100">
   <si>
     <t>Designator</t>
   </si>
@@ -80,6 +80,9 @@
     <t>Cdec1</t>
   </si>
   <si>
+    <t>CAP100</t>
+  </si>
+  <si>
     <t>Co11</t>
   </si>
   <si>
@@ -182,19 +185,16 @@
     <t>CMP-017-000066-1</t>
   </si>
   <si>
-    <t>JC1</t>
-  </si>
-  <si>
-    <t>JUMPER2</t>
-  </si>
-  <si>
-    <t>CMP-017-000037-1</t>
-  </si>
-  <si>
-    <t>JUMPER</t>
-  </si>
-  <si>
-    <t>JC2</t>
+    <t>Jds</t>
+  </si>
+  <si>
+    <t>SIP2</t>
+  </si>
+  <si>
+    <t>CMP-017-000004-1</t>
+  </si>
+  <si>
+    <t>CON2</t>
   </si>
   <si>
     <t>Jo1</t>
@@ -309,6 +309,24 @@
   </si>
   <si>
     <t>E55/28/21</t>
+  </si>
+  <si>
+    <t>TPfb</t>
+  </si>
+  <si>
+    <t>TPTH</t>
+  </si>
+  <si>
+    <t>CMP-015-000000-1</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>TPosc</t>
+  </si>
+  <si>
+    <t>TPx</t>
   </si>
   <si>
     <t>U1</t>
@@ -696,8 +714,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC9C2A5-4B28-4458-8311-C3AD3E26F7F2}">
-  <dimension ref="A1:E45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA3C293-7117-4333-A599-6FF2A3568FF8}">
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -780,7 +798,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -794,7 +812,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -806,46 +824,46 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
@@ -857,12 +875,12 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>6</v>
@@ -874,63 +892,63 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>6</v>
@@ -945,7 +963,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>6</v>
@@ -960,7 +978,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>6</v>
@@ -977,7 +995,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
@@ -989,52 +1007,52 @@
         <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1043,30 +1061,30 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1075,47 +1093,47 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1126,24 +1144,24 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>56</v>
@@ -1160,41 +1178,41 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>64</v>
@@ -1206,12 +1224,12 @@
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>64</v>
@@ -1228,13 +1246,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -1245,24 +1263,24 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>64</v>
@@ -1274,12 +1292,12 @@
         <v>1</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>64</v>
@@ -1291,12 +1309,12 @@
         <v>1</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>64</v>
@@ -1313,13 +1331,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
@@ -1330,7 +1348,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>64</v>
@@ -1347,56 +1365,56 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>71</v>
@@ -1408,44 +1426,46 @@
         <v>1</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D44" s="1">
         <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>91</v>
@@ -1458,6 +1478,40 @@
       </c>
       <c r="E45" s="2" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>